<commit_message>
Finalizacion de la pantalal de lista sin el eliminar
</commit_message>
<xml_diff>
--- a/documents/bdd/Data_Diccitionary.xlsx
+++ b/documents/bdd/Data_Diccitionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\Repositorios\gitHubRccs09\seguimiento\seguimiento\documents\bdd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C8DCD3-9B96-4E95-A7F6-435EBE368A34}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A279CFB-BBDF-4167-973E-650106B232DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{E157C3C5-B5A8-41AD-AEED-18F1476C04A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="9" xr2:uid="{E157C3C5-B5A8-41AD-AEED-18F1476C04A5}"/>
   </bookViews>
   <sheets>
     <sheet name="provider" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,10 @@
     <sheet name="component" sheetId="5" r:id="rId5"/>
     <sheet name="ticket" sheetId="6" r:id="rId6"/>
     <sheet name="ticket_detail" sheetId="7" r:id="rId7"/>
-    <sheet name="ticket_qa" sheetId="8" r:id="rId8"/>
-    <sheet name="ticket_prod" sheetId="9" r:id="rId9"/>
+    <sheet name="detail_qa" sheetId="10" r:id="rId8"/>
+    <sheet name="ticket_qa" sheetId="8" r:id="rId9"/>
+    <sheet name="detail_prod" sheetId="11" r:id="rId10"/>
+    <sheet name="ticket_prod" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -328,12 +330,24 @@
 4.- cerrado
 5.- Error de ejecucion</t>
   </si>
+  <si>
+    <t>dqa_id</t>
+  </si>
+  <si>
+    <t>id del ticket de QA</t>
+  </si>
+  <si>
+    <t>dprod_id</t>
+  </si>
+  <si>
+    <t>id del ticket de produccion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +357,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -385,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -417,6 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,6 +818,205 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE75D0DB-87AE-4C83-A78B-BA650FF19F50}">
+  <dimension ref="B2:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F47752-ED26-4820-A148-EEA297FD27DE}">
+  <dimension ref="B2:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="11"/>
+    <col min="2" max="2" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50088830-B550-46BE-91B6-E3229ED00A66}">
   <dimension ref="B2:E6"/>
@@ -1295,7 +1517,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,11 +1676,87 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB777E-7020-4A72-96A4-2A3582B67F20}">
-  <dimension ref="B2:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF3943-024E-4A95-9C6C-5C69019B12D2}">
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDB777E-7020-4A72-96A4-2A3582B67F20}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,155 +1881,6 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F47752-ED26-4820-A148-EEA297FD27DE}">
-  <dimension ref="B2:E9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.42578125" style="11"/>
-    <col min="2" max="2" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="87" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="11"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>